<commit_message>
[yerim] relic 의 효과타입 effect id 로 변경 적용
</commit_message>
<xml_diff>
--- a/GameData/Excel/relic.xlsx
+++ b/GameData/Excel/relic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\Go.D.Taekwon\GameData\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yerim\portfolio_Game\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC568E6-4AF2-4549-9F95-997C6FA30D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8EF79B-B0C0-483D-A5BD-001990F50CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="46296" windowHeight="25680" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="relic" sheetId="1" r:id="rId1"/>
@@ -98,39 +98,21 @@
     <t>condition_logic</t>
   </si>
   <si>
-    <t>relic_effect_1</t>
-  </si>
-  <si>
     <t>효과 1</t>
   </si>
   <si>
-    <t>effect_value_1</t>
-  </si>
-  <si>
     <t>효과 1 관련 값</t>
   </si>
   <si>
-    <t>relic_effect_2</t>
-  </si>
-  <si>
     <t>효과 2</t>
   </si>
   <si>
-    <t>effect_value_2</t>
-  </si>
-  <si>
     <t>효과 2 관련 값</t>
   </si>
   <si>
-    <t>relic_effect_3</t>
-  </si>
-  <si>
     <t>효과 3</t>
   </si>
   <si>
-    <t>effect_value_3</t>
-  </si>
-  <si>
     <t>효과 3 관련 값</t>
   </si>
   <si>
@@ -194,30 +176,6 @@
   </si>
   <si>
     <t>self</t>
-  </si>
-  <si>
-    <t>target_3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>target_count_3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>target_count_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>target_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>target_count_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>target_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>발동 조건 1, 2의 처리 조건 (AND, OR)</t>
@@ -262,6 +220,54 @@
   <si>
     <t>효과
 (spell_effect의 effect_id 참조)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#target_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#target_count_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#relic_effect_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#effect_value_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#target_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#target_count_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#relic_effect_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#effect_value_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#target_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#target_count_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#relic_effect_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#effect_value_3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -713,41 +719,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
   <dimension ref="A1:W197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.19921875" style="3" customWidth="1"/>
-    <col min="3" max="6" width="19.3984375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.8984375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.3984375" style="3" customWidth="1"/>
-    <col min="9" max="10" width="10.8984375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="40.09765625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="19.3984375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.8984375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="19.3984375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.8984375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="19.3984375" style="3" customWidth="1"/>
-    <col min="17" max="17" width="10.8984375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="19.3984375" style="3" customWidth="1"/>
-    <col min="19" max="19" width="10.8984375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="19.3984375" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.8984375" style="3" customWidth="1"/>
-    <col min="22" max="22" width="19.3984375" style="3" customWidth="1"/>
-    <col min="23" max="23" width="10.8984375" style="3" customWidth="1"/>
-    <col min="24" max="16384" width="8.69921875" style="3"/>
+    <col min="2" max="2" width="8.25" style="3" customWidth="1"/>
+    <col min="3" max="6" width="19.375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.375" style="3" customWidth="1"/>
+    <col min="9" max="10" width="10.875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="40.125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="19.375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="19.375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="19.375" style="3" customWidth="1"/>
+    <col min="17" max="17" width="10.875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="19.375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="10.875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="13.25" style="3" customWidth="1"/>
+    <col min="21" max="21" width="10.875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="19.375" style="3" customWidth="1"/>
+    <col min="23" max="23" width="10.875" style="3" customWidth="1"/>
+    <col min="24" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" s="8" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>5</v>
@@ -774,46 +780,46 @@
         <v>19</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>56</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -842,54 +848,54 @@
         <v>18</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="T2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:23" s="5" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
@@ -901,585 +907,585 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="U3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="W3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I4" s="3">
         <v>20</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M4" s="3">
         <v>1</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="O4" s="3">
         <v>5</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="3">
         <v>1</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="S4" s="3">
         <v>10</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="U4" s="3">
         <v>1</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="W4" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G5" s="3">
         <v>10</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I5" s="3">
         <v>90</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="K5" s="12">
         <v>10201</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M5" s="3">
         <v>1</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O5" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="K84" s="13"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="10"/>
       <c r="K167" s="13"/>
     </row>
-    <row r="168" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
       <c r="K168" s="13"/>
     </row>
-    <row r="169" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="10"/>
       <c r="K169" s="13"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" s="1"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" s="1"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" s="1"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" s="1"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" s="1"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" s="1"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" s="1"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" s="1"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" s="1"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" s="1"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" s="1"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" s="1"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B189" s="1"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" s="1"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" s="1"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" s="1"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" s="1"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" s="1"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" s="1"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" s="1"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" s="1"/>
     </row>
   </sheetData>

</xml_diff>